<commit_message>
Add sql project to repo
</commit_message>
<xml_diff>
--- a/homework18 excel/Students.XLSX
+++ b/homework18 excel/Students.XLSX
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Id</t>
   </si>
@@ -52,12 +52,6 @@
   </si>
   <si>
     <t>Maqa</t>
-  </si>
-  <si>
-    <t>Mahmud</t>
-  </si>
-  <si>
-    <t>Eliyev</t>
   </si>
   <si>
     <t>Musa</t>
@@ -379,7 +373,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
@@ -459,7 +453,7 @@
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>11</v>
@@ -468,20 +462,6 @@
         <v>12</v>
       </c>
       <c r="D6" s="0">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="0">
-        <v>9</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="0">
         <v>11</v>
       </c>
     </row>

</xml_diff>